<commit_message>
modifiche interfaccia home a metà
</commit_message>
<xml_diff>
--- a/vodafone-selenium-form/excelVodafoneOutPut.xlsx
+++ b/vodafone-selenium-form/excelVodafoneOutPut.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t xml:space="preserve">informazioni</t>
   </si>
@@ -143,15 +143,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>00118909</t>
-  </si>
-  <si>
-    <t>00118910</t>
-  </si>
-  <si>
-    <t>00118911</t>
   </si>
 </sst>
 </file>
@@ -436,7 +427,7 @@
         <v>34</v>
       </c>
       <c r="S3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -495,7 +486,7 @@
         <v>34</v>
       </c>
       <c r="S4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -554,7 +545,7 @@
         <v>34</v>
       </c>
       <c r="S5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>